<commit_message>
daily updates and begining of location coding
</commit_message>
<xml_diff>
--- a/Estimator_Worksheet-1.xlsx
+++ b/Estimator_Worksheet-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kijah\Documents\Data_Bootcamp\Estimator_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C1B2EB3-BE27-42AA-A7F1-ABF3AE538EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{29BBB91C-0CFB-43EB-9243-899EC6FF6B43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" firstSheet="11" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary - Rates" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,8 @@
     <sheet name="Cleaned_Data3" sheetId="12" r:id="rId12"/>
     <sheet name="Working_Table4" sheetId="13" r:id="rId13"/>
     <sheet name="Cleaned_Data4" sheetId="14" r:id="rId14"/>
+    <sheet name="Working_Table5" sheetId="15" r:id="rId15"/>
+    <sheet name="Cleaned_Data5" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -47,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1597" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1914" uniqueCount="166">
   <si>
     <t>Sales Tax</t>
   </si>
@@ -539,6 +541,12 @@
   </si>
   <si>
     <t>https://www.supplyworks.com/Sku/2487704/southwire-250-ft-122-solid-romex-simpull-cu-nm-b-wg-wire-032886163050-28828255</t>
+  </si>
+  <si>
+    <t>11/03/2022 10:47:48</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/p/1203573345</t>
   </si>
 </sst>
 </file>
@@ -549,7 +557,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -725,6 +733,11 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -794,7 +807,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -1109,12 +1122,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1248,31 +1276,17 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="17" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1285,6 +1299,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4497,7 +4528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:G47"/>
     </sheetView>
   </sheetViews>
@@ -5588,6 +5619,1497 @@
       </c>
       <c r="G47" t="s">
         <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.9296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="110.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B1" s="75" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="75" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="75" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="75" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="75" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" s="75">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" s="75">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" s="75">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4">
+        <v>17.55</v>
+      </c>
+      <c r="E4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" s="75">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5">
+        <v>3.98</v>
+      </c>
+      <c r="E5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" s="75">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6">
+        <v>2.98</v>
+      </c>
+      <c r="E6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" s="75">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" s="75">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8">
+        <v>2.1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" s="75">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" t="s">
+        <v>148</v>
+      </c>
+      <c r="G9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" s="75">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10">
+        <v>1.6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" t="s">
+        <v>76</v>
+      </c>
+      <c r="G10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" s="75">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11">
+        <v>84.99</v>
+      </c>
+      <c r="E11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" s="75">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12">
+        <v>158</v>
+      </c>
+      <c r="E12" t="s">
+        <v>107</v>
+      </c>
+      <c r="F12" t="s">
+        <v>154</v>
+      </c>
+      <c r="G12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" s="75">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" t="s">
+        <v>140</v>
+      </c>
+      <c r="D13">
+        <v>149</v>
+      </c>
+      <c r="E13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" t="s">
+        <v>146</v>
+      </c>
+      <c r="G13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" s="75">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14">
+        <v>279</v>
+      </c>
+      <c r="E14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" s="75">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15">
+        <v>60</v>
+      </c>
+      <c r="E15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" s="75">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16">
+        <v>99</v>
+      </c>
+      <c r="E16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" t="s">
+        <v>91</v>
+      </c>
+      <c r="G16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" s="75">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17">
+        <v>145</v>
+      </c>
+      <c r="E17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" t="s">
+        <v>94</v>
+      </c>
+      <c r="G17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:G46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.9296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="119.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B1" s="75" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="75" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="75" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="75" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="75" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" s="75">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2">
+        <v>20.62</v>
+      </c>
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" s="75">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3">
+        <v>17.55</v>
+      </c>
+      <c r="E3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" s="75">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4">
+        <v>11.91</v>
+      </c>
+      <c r="E4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" s="75">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5">
+        <v>10.47</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" s="75">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" s="75">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7">
+        <v>3.98</v>
+      </c>
+      <c r="E7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" t="s">
+        <v>102</v>
+      </c>
+      <c r="G7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" s="75">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8">
+        <v>5.99</v>
+      </c>
+      <c r="E8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" s="75">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9">
+        <v>5.99</v>
+      </c>
+      <c r="E9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F9" t="s">
+        <v>104</v>
+      </c>
+      <c r="G9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" s="75">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10">
+        <v>2.1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F10" t="s">
+        <v>105</v>
+      </c>
+      <c r="G10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" s="75">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="E11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" s="75">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" s="75">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13">
+        <v>3.98</v>
+      </c>
+      <c r="E13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" t="s">
+        <v>102</v>
+      </c>
+      <c r="G13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" s="75">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14">
+        <v>8.5399999999999991</v>
+      </c>
+      <c r="E14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" s="75">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" t="s">
+        <v>117</v>
+      </c>
+      <c r="G15" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" s="75">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16">
+        <v>5.99</v>
+      </c>
+      <c r="E16" t="s">
+        <v>103</v>
+      </c>
+      <c r="F16" t="s">
+        <v>118</v>
+      </c>
+      <c r="G16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" s="75">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17">
+        <v>20</v>
+      </c>
+      <c r="E17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" t="s">
+        <v>148</v>
+      </c>
+      <c r="G17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" s="75">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18">
+        <v>1.6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" t="s">
+        <v>120</v>
+      </c>
+      <c r="G18" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" s="75">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19">
+        <v>1.99</v>
+      </c>
+      <c r="E19" t="s">
+        <v>75</v>
+      </c>
+      <c r="F19" t="s">
+        <v>76</v>
+      </c>
+      <c r="G19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20" s="75">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20">
+        <v>2.98</v>
+      </c>
+      <c r="E20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" s="75">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21">
+        <v>3.66</v>
+      </c>
+      <c r="E21" t="s">
+        <v>111</v>
+      </c>
+      <c r="F21" t="s">
+        <v>119</v>
+      </c>
+      <c r="G21" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" s="75">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22">
+        <v>5.99</v>
+      </c>
+      <c r="E22" t="s">
+        <v>103</v>
+      </c>
+      <c r="F22" t="s">
+        <v>121</v>
+      </c>
+      <c r="G22" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23" s="75">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23">
+        <v>2.98</v>
+      </c>
+      <c r="E23" t="s">
+        <v>149</v>
+      </c>
+      <c r="F23" t="s">
+        <v>150</v>
+      </c>
+      <c r="G23" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A24" s="75">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24">
+        <v>75.88</v>
+      </c>
+      <c r="E24" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" t="s">
+        <v>122</v>
+      </c>
+      <c r="G24" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A25" s="75">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25">
+        <v>106.54</v>
+      </c>
+      <c r="E25" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" t="s">
+        <v>88</v>
+      </c>
+      <c r="G25" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A26" s="75">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26">
+        <v>64.989999999999995</v>
+      </c>
+      <c r="E26" t="s">
+        <v>157</v>
+      </c>
+      <c r="F26" t="s">
+        <v>158</v>
+      </c>
+      <c r="G26" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A27" s="75">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27">
+        <v>60</v>
+      </c>
+      <c r="E27" t="s">
+        <v>107</v>
+      </c>
+      <c r="F27" t="s">
+        <v>165</v>
+      </c>
+      <c r="G27" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A28" s="75">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28">
+        <v>99</v>
+      </c>
+      <c r="E28" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G28" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A29" s="75">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29">
+        <v>117</v>
+      </c>
+      <c r="E29" t="s">
+        <v>103</v>
+      </c>
+      <c r="F29" t="s">
+        <v>125</v>
+      </c>
+      <c r="G29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A30" s="75">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30">
+        <v>120.61</v>
+      </c>
+      <c r="E30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F30" t="s">
+        <v>91</v>
+      </c>
+      <c r="G30" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A31" s="75">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31">
+        <v>145</v>
+      </c>
+      <c r="E31" t="s">
+        <v>62</v>
+      </c>
+      <c r="F31" t="s">
+        <v>126</v>
+      </c>
+      <c r="G31" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A32" s="75">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32">
+        <v>155.99</v>
+      </c>
+      <c r="E32" t="s">
+        <v>58</v>
+      </c>
+      <c r="F32" t="s">
+        <v>94</v>
+      </c>
+      <c r="G32" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A33" s="75">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" t="s">
+        <v>78</v>
+      </c>
+      <c r="D33">
+        <v>118</v>
+      </c>
+      <c r="E33" t="s">
+        <v>62</v>
+      </c>
+      <c r="F33" t="s">
+        <v>144</v>
+      </c>
+      <c r="G33" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A34" s="75">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34">
+        <v>114</v>
+      </c>
+      <c r="E34" t="s">
+        <v>58</v>
+      </c>
+      <c r="F34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G34" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A35" s="75">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35">
+        <v>118</v>
+      </c>
+      <c r="E35" t="s">
+        <v>103</v>
+      </c>
+      <c r="F35" t="s">
+        <v>145</v>
+      </c>
+      <c r="G35" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A36" s="75">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" t="s">
+        <v>78</v>
+      </c>
+      <c r="D36">
+        <v>111.07</v>
+      </c>
+      <c r="E36" t="s">
+        <v>107</v>
+      </c>
+      <c r="F36" t="s">
+        <v>129</v>
+      </c>
+      <c r="G36" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A37" s="75">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37">
+        <v>84.99</v>
+      </c>
+      <c r="E37" t="s">
+        <v>130</v>
+      </c>
+      <c r="F37" t="s">
+        <v>131</v>
+      </c>
+      <c r="G37" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A38" s="75">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38">
+        <v>158</v>
+      </c>
+      <c r="E38" t="s">
+        <v>62</v>
+      </c>
+      <c r="F38" t="s">
+        <v>82</v>
+      </c>
+      <c r="G38" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A39" s="75">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" t="s">
+        <v>81</v>
+      </c>
+      <c r="D39">
+        <v>159</v>
+      </c>
+      <c r="E39" t="s">
+        <v>103</v>
+      </c>
+      <c r="F39" t="s">
+        <v>134</v>
+      </c>
+      <c r="G39" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A40" s="75">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40" t="s">
+        <v>81</v>
+      </c>
+      <c r="D40">
+        <v>172.22</v>
+      </c>
+      <c r="E40" t="s">
+        <v>107</v>
+      </c>
+      <c r="F40" t="s">
+        <v>154</v>
+      </c>
+      <c r="G40" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A41" s="75">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41">
+        <v>215</v>
+      </c>
+      <c r="E41" t="s">
+        <v>161</v>
+      </c>
+      <c r="F41" t="s">
+        <v>162</v>
+      </c>
+      <c r="G41" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A42" s="75">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>139</v>
+      </c>
+      <c r="C42" t="s">
+        <v>140</v>
+      </c>
+      <c r="D42">
+        <v>149</v>
+      </c>
+      <c r="E42" t="s">
+        <v>62</v>
+      </c>
+      <c r="F42" t="s">
+        <v>146</v>
+      </c>
+      <c r="G42" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A43" s="75">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>139</v>
+      </c>
+      <c r="C43" t="s">
+        <v>140</v>
+      </c>
+      <c r="D43">
+        <v>149</v>
+      </c>
+      <c r="E43" t="s">
+        <v>103</v>
+      </c>
+      <c r="F43" t="s">
+        <v>151</v>
+      </c>
+      <c r="G43" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A44" s="75">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" t="s">
+        <v>84</v>
+      </c>
+      <c r="D44">
+        <v>279</v>
+      </c>
+      <c r="E44" t="s">
+        <v>62</v>
+      </c>
+      <c r="F44" t="s">
+        <v>85</v>
+      </c>
+      <c r="G44" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A45" s="75">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" t="s">
+        <v>84</v>
+      </c>
+      <c r="D45">
+        <v>289</v>
+      </c>
+      <c r="E45" t="s">
+        <v>103</v>
+      </c>
+      <c r="F45" t="s">
+        <v>135</v>
+      </c>
+      <c r="G45" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A46" s="75">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>83</v>
+      </c>
+      <c r="C46" t="s">
+        <v>84</v>
+      </c>
+      <c r="D46">
+        <v>339.09</v>
+      </c>
+      <c r="E46" t="s">
+        <v>136</v>
+      </c>
+      <c r="F46" t="s">
+        <v>137</v>
+      </c>
+      <c r="G46" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -5830,13 +7352,13 @@
       <c r="P8" s="63"/>
     </row>
     <row r="9" spans="1:16" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="75" t="s">
+      <c r="A9" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="76"/>
-      <c r="C9" s="76"/>
-      <c r="D9" s="76"/>
-      <c r="E9" s="77"/>
+      <c r="B9" s="77"/>
+      <c r="C9" s="77"/>
+      <c r="D9" s="77"/>
+      <c r="E9" s="87"/>
       <c r="F9" s="9"/>
       <c r="G9" s="51">
         <f t="shared" si="1"/>
@@ -5859,14 +7381,14 @@
         <v>11</v>
       </c>
       <c r="D10" s="14"/>
-      <c r="E10" s="78" t="s">
+      <c r="E10" s="88" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="54" t="str">
         <f>C10</f>
         <v>TOTAL</v>
       </c>
-      <c r="G10" s="80" t="s">
+      <c r="G10" s="90" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="63"/>
@@ -5886,11 +7408,11 @@
         <v>14</v>
       </c>
       <c r="D11" s="55"/>
-      <c r="E11" s="79"/>
+      <c r="E11" s="89"/>
       <c r="F11" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="81"/>
+      <c r="G11" s="79"/>
       <c r="H11" s="63"/>
       <c r="I11" s="63"/>
       <c r="J11" s="63"/>
@@ -5902,59 +7424,59 @@
       <c r="P11" s="63"/>
     </row>
     <row r="12" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="82" t="s">
+      <c r="A12" s="91" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="83">
+      <c r="B12" s="92">
         <f t="shared" ref="B12:G12" si="2">SUM(B2:B8)</f>
         <v>0</v>
       </c>
-      <c r="C12" s="83">
+      <c r="C12" s="92">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D12" s="83">
+      <c r="D12" s="92">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E12" s="83">
+      <c r="E12" s="92">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F12" s="83">
+      <c r="F12" s="92">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G12" s="86">
+      <c r="G12" s="80">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H12" s="88" t="s">
+      <c r="H12" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="81"/>
-      <c r="J12" s="81"/>
-      <c r="K12" s="81"/>
-      <c r="L12" s="81"/>
-      <c r="M12" s="81"/>
+      <c r="I12" s="79"/>
+      <c r="J12" s="79"/>
+      <c r="K12" s="79"/>
+      <c r="L12" s="79"/>
+      <c r="M12" s="79"/>
       <c r="N12" s="63"/>
       <c r="O12" s="63"/>
       <c r="P12" s="63"/>
     </row>
     <row r="13" spans="1:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="81"/>
-      <c r="B13" s="81"/>
-      <c r="C13" s="81"/>
-      <c r="D13" s="81"/>
-      <c r="E13" s="81"/>
-      <c r="F13" s="81"/>
-      <c r="G13" s="87"/>
-      <c r="H13" s="89"/>
-      <c r="I13" s="81"/>
-      <c r="J13" s="81"/>
-      <c r="K13" s="81"/>
-      <c r="L13" s="81"/>
-      <c r="M13" s="81"/>
+      <c r="A13" s="79"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="79"/>
+      <c r="D13" s="79"/>
+      <c r="E13" s="79"/>
+      <c r="F13" s="79"/>
+      <c r="G13" s="81"/>
+      <c r="H13" s="83"/>
+      <c r="I13" s="79"/>
+      <c r="J13" s="79"/>
+      <c r="K13" s="79"/>
+      <c r="L13" s="79"/>
+      <c r="M13" s="79"/>
       <c r="N13" s="63"/>
       <c r="O13" s="63"/>
       <c r="P13" s="63"/>
@@ -6019,10 +7541,10 @@
       <c r="B18" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="90"/>
-      <c r="D18" s="91"/>
-      <c r="E18" s="91"/>
-      <c r="F18" s="91"/>
+      <c r="C18" s="84"/>
+      <c r="D18" s="85"/>
+      <c r="E18" s="85"/>
+      <c r="F18" s="85"/>
       <c r="G18" s="63"/>
       <c r="H18" s="63"/>
       <c r="I18" s="63"/>
@@ -6039,10 +7561,10 @@
       <c r="B19" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="84"/>
-      <c r="D19" s="76"/>
-      <c r="E19" s="76"/>
-      <c r="F19" s="76"/>
+      <c r="C19" s="76"/>
+      <c r="D19" s="77"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="77"/>
       <c r="G19" s="63"/>
       <c r="H19" s="63"/>
       <c r="I19" s="63"/>
@@ -6059,15 +7581,15 @@
       <c r="B20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="90"/>
-      <c r="D20" s="91"/>
-      <c r="E20" s="91"/>
-      <c r="F20" s="91"/>
-      <c r="G20" s="91"/>
-      <c r="H20" s="91"/>
-      <c r="I20" s="91"/>
-      <c r="J20" s="91"/>
-      <c r="K20" s="91"/>
+      <c r="C20" s="84"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="85"/>
+      <c r="F20" s="85"/>
+      <c r="G20" s="85"/>
+      <c r="H20" s="85"/>
+      <c r="I20" s="85"/>
+      <c r="J20" s="85"/>
+      <c r="K20" s="85"/>
       <c r="L20" s="63"/>
       <c r="M20" s="63"/>
       <c r="N20" s="63"/>
@@ -6079,10 +7601,10 @@
       <c r="B21" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="84"/>
-      <c r="D21" s="76"/>
-      <c r="E21" s="76"/>
-      <c r="F21" s="76"/>
+      <c r="C21" s="76"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="77"/>
       <c r="G21" s="67"/>
       <c r="H21" s="63"/>
       <c r="I21" s="63"/>
@@ -6112,14 +7634,14 @@
     <row r="23" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A23" s="63"/>
       <c r="B23" s="63"/>
-      <c r="C23" s="85" t="s">
+      <c r="C23" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="81"/>
-      <c r="E23" s="81"/>
-      <c r="F23" s="81"/>
-      <c r="G23" s="81"/>
-      <c r="H23" s="81"/>
+      <c r="D23" s="79"/>
+      <c r="E23" s="79"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="79"/>
       <c r="I23" s="63"/>
       <c r="J23" s="63"/>
       <c r="K23" s="63"/>
@@ -6132,12 +7654,12 @@
     <row r="24" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A24" s="63"/>
       <c r="B24" s="63"/>
-      <c r="C24" s="81"/>
-      <c r="D24" s="81"/>
-      <c r="E24" s="81"/>
-      <c r="F24" s="81"/>
-      <c r="G24" s="81"/>
-      <c r="H24" s="81"/>
+      <c r="C24" s="79"/>
+      <c r="D24" s="79"/>
+      <c r="E24" s="79"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="79"/>
       <c r="I24" s="63"/>
       <c r="J24" s="63"/>
       <c r="K24" s="63"/>
@@ -6150,12 +7672,12 @@
     <row r="25" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A25" s="63"/>
       <c r="B25" s="63"/>
-      <c r="C25" s="81"/>
-      <c r="D25" s="81"/>
-      <c r="E25" s="81"/>
-      <c r="F25" s="81"/>
-      <c r="G25" s="81"/>
-      <c r="H25" s="81"/>
+      <c r="C25" s="79"/>
+      <c r="D25" s="79"/>
+      <c r="E25" s="79"/>
+      <c r="F25" s="79"/>
+      <c r="G25" s="79"/>
+      <c r="H25" s="79"/>
       <c r="I25" s="63"/>
       <c r="J25" s="63"/>
       <c r="K25" s="63"/>
@@ -6185,13 +7707,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C23:H25"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:M13"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:K20"/>
     <mergeCell ref="A9:E9"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="G10:G11"/>
@@ -6201,6 +7716,13 @@
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C23:H25"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:M13"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:K20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added graph images, and daily updates. We're at 735 rows!
</commit_message>
<xml_diff>
--- a/Estimator_Worksheet-1.xlsx
+++ b/Estimator_Worksheet-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kijah\Documents\Data_Bootcamp\Estimator_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2CD3A919-33A1-469D-901D-AAC93CD5365E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC029E6C-E6BE-4797-B585-402F3DF23217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" firstSheet="15" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" firstSheet="17" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary - Rates" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,8 @@
     <sheet name="Cleaned_Data6" sheetId="18" r:id="rId18"/>
     <sheet name="Working_Table7" sheetId="19" r:id="rId19"/>
     <sheet name="Cleaned_Data7" sheetId="20" r:id="rId20"/>
+    <sheet name="Working_Table8" sheetId="21" r:id="rId21"/>
+    <sheet name="Cleaned_Data8" sheetId="22" r:id="rId22"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -53,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2595" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2932" uniqueCount="182">
   <si>
     <t>Sales Tax</t>
   </si>
@@ -591,6 +593,15 @@
   <si>
     <t>https://www.ebay.com/itm/203860011450</t>
   </si>
+  <si>
+    <t>11/06/2022 08:48:53</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/194605434077</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/b/14-2-Romex-Indiana-OTHER-Industrial-Wires-Cables/92078/bn_7022085018</t>
+  </si>
 </sst>
 </file>
 
@@ -600,7 +611,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -791,6 +802,11 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -860,7 +876,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -1220,12 +1236,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1368,31 +1399,17 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="17" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1405,6 +1422,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9396,13 +9430,13 @@
       <c r="P8" s="63"/>
     </row>
     <row r="9" spans="1:16" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="78" t="s">
+      <c r="A9" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="80"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="90"/>
       <c r="F9" s="9"/>
       <c r="G9" s="51">
         <f t="shared" si="1"/>
@@ -9425,14 +9459,14 @@
         <v>11</v>
       </c>
       <c r="D10" s="14"/>
-      <c r="E10" s="81" t="s">
+      <c r="E10" s="91" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="54" t="str">
         <f>C10</f>
         <v>TOTAL</v>
       </c>
-      <c r="G10" s="83" t="s">
+      <c r="G10" s="93" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="63"/>
@@ -9452,11 +9486,11 @@
         <v>14</v>
       </c>
       <c r="D11" s="55"/>
-      <c r="E11" s="82"/>
+      <c r="E11" s="92"/>
       <c r="F11" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="84"/>
+      <c r="G11" s="82"/>
       <c r="H11" s="63"/>
       <c r="I11" s="63"/>
       <c r="J11" s="63"/>
@@ -9468,59 +9502,59 @@
       <c r="P11" s="63"/>
     </row>
     <row r="12" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="85" t="s">
+      <c r="A12" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="86">
+      <c r="B12" s="95">
         <f t="shared" ref="B12:G12" si="2">SUM(B2:B8)</f>
         <v>0</v>
       </c>
-      <c r="C12" s="86">
+      <c r="C12" s="95">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D12" s="86">
+      <c r="D12" s="95">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E12" s="86">
+      <c r="E12" s="95">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F12" s="86">
+      <c r="F12" s="95">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G12" s="89">
+      <c r="G12" s="83">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H12" s="91" t="s">
+      <c r="H12" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="84"/>
-      <c r="J12" s="84"/>
-      <c r="K12" s="84"/>
-      <c r="L12" s="84"/>
-      <c r="M12" s="84"/>
+      <c r="I12" s="82"/>
+      <c r="J12" s="82"/>
+      <c r="K12" s="82"/>
+      <c r="L12" s="82"/>
+      <c r="M12" s="82"/>
       <c r="N12" s="63"/>
       <c r="O12" s="63"/>
       <c r="P12" s="63"/>
     </row>
     <row r="13" spans="1:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="84"/>
-      <c r="B13" s="84"/>
-      <c r="C13" s="84"/>
-      <c r="D13" s="84"/>
-      <c r="E13" s="84"/>
-      <c r="F13" s="84"/>
-      <c r="G13" s="90"/>
-      <c r="H13" s="92"/>
-      <c r="I13" s="84"/>
-      <c r="J13" s="84"/>
-      <c r="K13" s="84"/>
-      <c r="L13" s="84"/>
-      <c r="M13" s="84"/>
+      <c r="A13" s="82"/>
+      <c r="B13" s="82"/>
+      <c r="C13" s="82"/>
+      <c r="D13" s="82"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="82"/>
+      <c r="G13" s="84"/>
+      <c r="H13" s="86"/>
+      <c r="I13" s="82"/>
+      <c r="J13" s="82"/>
+      <c r="K13" s="82"/>
+      <c r="L13" s="82"/>
+      <c r="M13" s="82"/>
       <c r="N13" s="63"/>
       <c r="O13" s="63"/>
       <c r="P13" s="63"/>
@@ -9585,10 +9619,10 @@
       <c r="B18" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="93"/>
-      <c r="D18" s="94"/>
-      <c r="E18" s="94"/>
-      <c r="F18" s="94"/>
+      <c r="C18" s="87"/>
+      <c r="D18" s="88"/>
+      <c r="E18" s="88"/>
+      <c r="F18" s="88"/>
       <c r="G18" s="63"/>
       <c r="H18" s="63"/>
       <c r="I18" s="63"/>
@@ -9605,10 +9639,10 @@
       <c r="B19" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="87"/>
-      <c r="D19" s="79"/>
-      <c r="E19" s="79"/>
-      <c r="F19" s="79"/>
+      <c r="C19" s="79"/>
+      <c r="D19" s="80"/>
+      <c r="E19" s="80"/>
+      <c r="F19" s="80"/>
       <c r="G19" s="63"/>
       <c r="H19" s="63"/>
       <c r="I19" s="63"/>
@@ -9625,15 +9659,15 @@
       <c r="B20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="93"/>
-      <c r="D20" s="94"/>
-      <c r="E20" s="94"/>
-      <c r="F20" s="94"/>
-      <c r="G20" s="94"/>
-      <c r="H20" s="94"/>
-      <c r="I20" s="94"/>
-      <c r="J20" s="94"/>
-      <c r="K20" s="94"/>
+      <c r="C20" s="87"/>
+      <c r="D20" s="88"/>
+      <c r="E20" s="88"/>
+      <c r="F20" s="88"/>
+      <c r="G20" s="88"/>
+      <c r="H20" s="88"/>
+      <c r="I20" s="88"/>
+      <c r="J20" s="88"/>
+      <c r="K20" s="88"/>
       <c r="L20" s="63"/>
       <c r="M20" s="63"/>
       <c r="N20" s="63"/>
@@ -9645,10 +9679,10 @@
       <c r="B21" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="87"/>
-      <c r="D21" s="79"/>
-      <c r="E21" s="79"/>
-      <c r="F21" s="79"/>
+      <c r="C21" s="79"/>
+      <c r="D21" s="80"/>
+      <c r="E21" s="80"/>
+      <c r="F21" s="80"/>
       <c r="G21" s="67"/>
       <c r="H21" s="63"/>
       <c r="I21" s="63"/>
@@ -9678,14 +9712,14 @@
     <row r="23" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A23" s="63"/>
       <c r="B23" s="63"/>
-      <c r="C23" s="88" t="s">
+      <c r="C23" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="84"/>
-      <c r="E23" s="84"/>
-      <c r="F23" s="84"/>
-      <c r="G23" s="84"/>
-      <c r="H23" s="84"/>
+      <c r="D23" s="82"/>
+      <c r="E23" s="82"/>
+      <c r="F23" s="82"/>
+      <c r="G23" s="82"/>
+      <c r="H23" s="82"/>
       <c r="I23" s="63"/>
       <c r="J23" s="63"/>
       <c r="K23" s="63"/>
@@ -9698,12 +9732,12 @@
     <row r="24" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A24" s="63"/>
       <c r="B24" s="63"/>
-      <c r="C24" s="84"/>
-      <c r="D24" s="84"/>
-      <c r="E24" s="84"/>
-      <c r="F24" s="84"/>
-      <c r="G24" s="84"/>
-      <c r="H24" s="84"/>
+      <c r="C24" s="82"/>
+      <c r="D24" s="82"/>
+      <c r="E24" s="82"/>
+      <c r="F24" s="82"/>
+      <c r="G24" s="82"/>
+      <c r="H24" s="82"/>
       <c r="I24" s="63"/>
       <c r="J24" s="63"/>
       <c r="K24" s="63"/>
@@ -9716,12 +9750,12 @@
     <row r="25" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A25" s="63"/>
       <c r="B25" s="63"/>
-      <c r="C25" s="84"/>
-      <c r="D25" s="84"/>
-      <c r="E25" s="84"/>
-      <c r="F25" s="84"/>
-      <c r="G25" s="84"/>
-      <c r="H25" s="84"/>
+      <c r="C25" s="82"/>
+      <c r="D25" s="82"/>
+      <c r="E25" s="82"/>
+      <c r="F25" s="82"/>
+      <c r="G25" s="82"/>
+      <c r="H25" s="82"/>
       <c r="I25" s="63"/>
       <c r="J25" s="63"/>
       <c r="K25" s="63"/>
@@ -9751,13 +9785,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C23:H25"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:M13"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:K20"/>
     <mergeCell ref="A9:E9"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="G10:G11"/>
@@ -9767,6 +9794,13 @@
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C23:H25"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:M13"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:K20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9776,7 +9810,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:G52"/>
     </sheetView>
   </sheetViews>
@@ -10982,6 +11016,1589 @@
       </c>
       <c r="G52" t="s">
         <v>176</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.9296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="110.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B1" s="78" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="78" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="78" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="78" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" s="78" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="78" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" s="78">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" s="78">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3">
+        <v>8.6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" s="78">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4">
+        <v>17.55</v>
+      </c>
+      <c r="E4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" s="78">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5">
+        <v>3.98</v>
+      </c>
+      <c r="E5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" s="78">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6">
+        <v>2.98</v>
+      </c>
+      <c r="E6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" s="78">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" s="78">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8">
+        <v>2.1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" s="78">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" t="s">
+        <v>148</v>
+      </c>
+      <c r="G9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" s="78">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10">
+        <v>1.6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" t="s">
+        <v>120</v>
+      </c>
+      <c r="G10" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" s="78">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11">
+        <v>111.07</v>
+      </c>
+      <c r="E11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" s="78">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12">
+        <v>158</v>
+      </c>
+      <c r="E12" t="s">
+        <v>107</v>
+      </c>
+      <c r="F12" t="s">
+        <v>180</v>
+      </c>
+      <c r="G12" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" s="78">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" t="s">
+        <v>140</v>
+      </c>
+      <c r="D13">
+        <v>149</v>
+      </c>
+      <c r="E13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" t="s">
+        <v>146</v>
+      </c>
+      <c r="G13" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" s="78">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14">
+        <v>289</v>
+      </c>
+      <c r="E14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" s="78">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15">
+        <v>75.989999999999995</v>
+      </c>
+      <c r="E15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" s="78">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16">
+        <v>106</v>
+      </c>
+      <c r="E16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" t="s">
+        <v>91</v>
+      </c>
+      <c r="G16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" s="78">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17">
+        <v>155.99</v>
+      </c>
+      <c r="E17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" t="s">
+        <v>94</v>
+      </c>
+      <c r="G17" t="s">
+        <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+  <dimension ref="A1:G50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.9296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="137.53125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B1" s="78" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="78" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="78" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="78" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" s="78" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="78" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" s="78">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2">
+        <v>20.62</v>
+      </c>
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" s="78">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3">
+        <v>17.55</v>
+      </c>
+      <c r="E3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" s="78">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4">
+        <v>11.91</v>
+      </c>
+      <c r="E4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" s="78">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5">
+        <v>10.47</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" s="78">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6">
+        <v>8.6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" s="78">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7">
+        <v>3.98</v>
+      </c>
+      <c r="E7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" t="s">
+        <v>102</v>
+      </c>
+      <c r="G7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" s="78">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8">
+        <v>8.5399999999999991</v>
+      </c>
+      <c r="E8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" s="78">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9">
+        <v>5.99</v>
+      </c>
+      <c r="E9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F9" t="s">
+        <v>104</v>
+      </c>
+      <c r="G9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" s="78">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10">
+        <v>2.1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F10" t="s">
+        <v>105</v>
+      </c>
+      <c r="G10" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" s="78">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11">
+        <v>9.99</v>
+      </c>
+      <c r="E11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F11" t="s">
+        <v>174</v>
+      </c>
+      <c r="G11" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" s="78">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12">
+        <v>7.22</v>
+      </c>
+      <c r="E12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" t="s">
+        <v>109</v>
+      </c>
+      <c r="G12" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" s="78">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13">
+        <v>5.99</v>
+      </c>
+      <c r="E13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G13" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" s="78">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="E14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" s="78">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15">
+        <v>5.88</v>
+      </c>
+      <c r="E15" t="s">
+        <v>111</v>
+      </c>
+      <c r="F15" t="s">
+        <v>112</v>
+      </c>
+      <c r="G15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" s="78">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16">
+        <v>5.88</v>
+      </c>
+      <c r="E16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" t="s">
+        <v>169</v>
+      </c>
+      <c r="G16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" s="78">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17">
+        <v>7.24</v>
+      </c>
+      <c r="E17" t="s">
+        <v>113</v>
+      </c>
+      <c r="F17" t="s">
+        <v>114</v>
+      </c>
+      <c r="G17" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" s="78">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" s="78">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19">
+        <v>3.98</v>
+      </c>
+      <c r="E19" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" t="s">
+        <v>102</v>
+      </c>
+      <c r="G19" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20" s="78">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20">
+        <v>8.5399999999999991</v>
+      </c>
+      <c r="E20" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" s="78">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E21" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" t="s">
+        <v>117</v>
+      </c>
+      <c r="G21" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" s="78">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22">
+        <v>5.99</v>
+      </c>
+      <c r="E22" t="s">
+        <v>103</v>
+      </c>
+      <c r="F22" t="s">
+        <v>118</v>
+      </c>
+      <c r="G22" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23" s="78">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23">
+        <v>20</v>
+      </c>
+      <c r="E23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" t="s">
+        <v>148</v>
+      </c>
+      <c r="G23" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A24" s="78">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24">
+        <v>6.45</v>
+      </c>
+      <c r="E24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F24" t="s">
+        <v>177</v>
+      </c>
+      <c r="G24" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A25" s="78">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25">
+        <v>1.6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" t="s">
+        <v>120</v>
+      </c>
+      <c r="G25" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A26" s="78">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26">
+        <v>2.98</v>
+      </c>
+      <c r="E26" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" t="s">
+        <v>63</v>
+      </c>
+      <c r="G26" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A27" s="78">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27">
+        <v>3.66</v>
+      </c>
+      <c r="E27" t="s">
+        <v>111</v>
+      </c>
+      <c r="F27" t="s">
+        <v>119</v>
+      </c>
+      <c r="G27" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A28" s="78">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28">
+        <v>5.99</v>
+      </c>
+      <c r="E28" t="s">
+        <v>103</v>
+      </c>
+      <c r="F28" t="s">
+        <v>121</v>
+      </c>
+      <c r="G28" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A29" s="78">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29">
+        <v>2.98</v>
+      </c>
+      <c r="E29" t="s">
+        <v>149</v>
+      </c>
+      <c r="F29" t="s">
+        <v>150</v>
+      </c>
+      <c r="G29" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A30" s="78">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" t="s">
+        <v>87</v>
+      </c>
+      <c r="D30">
+        <v>81.95</v>
+      </c>
+      <c r="E30" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" t="s">
+        <v>122</v>
+      </c>
+      <c r="G30" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A31" s="78">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" t="s">
+        <v>87</v>
+      </c>
+      <c r="D31">
+        <v>75.989999999999995</v>
+      </c>
+      <c r="E31" t="s">
+        <v>58</v>
+      </c>
+      <c r="F31" t="s">
+        <v>88</v>
+      </c>
+      <c r="G31" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A32" s="78">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" t="s">
+        <v>87</v>
+      </c>
+      <c r="D32">
+        <v>80</v>
+      </c>
+      <c r="E32" t="s">
+        <v>127</v>
+      </c>
+      <c r="F32" t="s">
+        <v>156</v>
+      </c>
+      <c r="G32" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A33" s="78">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33">
+        <v>445.81</v>
+      </c>
+      <c r="E33" t="s">
+        <v>107</v>
+      </c>
+      <c r="F33" t="s">
+        <v>178</v>
+      </c>
+      <c r="G33" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A34" s="78">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" t="s">
+        <v>90</v>
+      </c>
+      <c r="D34">
+        <v>106</v>
+      </c>
+      <c r="E34" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34" t="s">
+        <v>124</v>
+      </c>
+      <c r="G34" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A35" s="78">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35">
+        <v>109</v>
+      </c>
+      <c r="E35" t="s">
+        <v>103</v>
+      </c>
+      <c r="F35" t="s">
+        <v>125</v>
+      </c>
+      <c r="G35" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A36" s="78">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" t="s">
+        <v>90</v>
+      </c>
+      <c r="D36">
+        <v>114.95</v>
+      </c>
+      <c r="E36" t="s">
+        <v>58</v>
+      </c>
+      <c r="F36" t="s">
+        <v>91</v>
+      </c>
+      <c r="G36" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A37" s="78">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37">
+        <v>156</v>
+      </c>
+      <c r="E37" t="s">
+        <v>62</v>
+      </c>
+      <c r="F37" t="s">
+        <v>126</v>
+      </c>
+      <c r="G37" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A38" s="78">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38">
+        <v>155.99</v>
+      </c>
+      <c r="E38" t="s">
+        <v>58</v>
+      </c>
+      <c r="F38" t="s">
+        <v>94</v>
+      </c>
+      <c r="G38" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A39" s="78">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>92</v>
+      </c>
+      <c r="C39" t="s">
+        <v>93</v>
+      </c>
+      <c r="D39">
+        <v>165</v>
+      </c>
+      <c r="E39" t="s">
+        <v>127</v>
+      </c>
+      <c r="F39" t="s">
+        <v>128</v>
+      </c>
+      <c r="G39" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A40" s="78">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" t="s">
+        <v>78</v>
+      </c>
+      <c r="D40">
+        <v>115.22</v>
+      </c>
+      <c r="E40" t="s">
+        <v>58</v>
+      </c>
+      <c r="F40" t="s">
+        <v>79</v>
+      </c>
+      <c r="G40" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A41" s="78">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>77</v>
+      </c>
+      <c r="C41" t="s">
+        <v>78</v>
+      </c>
+      <c r="D41">
+        <v>118</v>
+      </c>
+      <c r="E41" t="s">
+        <v>103</v>
+      </c>
+      <c r="F41" t="s">
+        <v>145</v>
+      </c>
+      <c r="G41" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A42" s="78">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42" t="s">
+        <v>78</v>
+      </c>
+      <c r="D42">
+        <v>111.07</v>
+      </c>
+      <c r="E42" t="s">
+        <v>107</v>
+      </c>
+      <c r="F42" t="s">
+        <v>181</v>
+      </c>
+      <c r="G42" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A43" s="78">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43">
+        <v>158</v>
+      </c>
+      <c r="E43" t="s">
+        <v>62</v>
+      </c>
+      <c r="F43" t="s">
+        <v>82</v>
+      </c>
+      <c r="G43" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A44" s="78">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44">
+        <v>158</v>
+      </c>
+      <c r="E44" t="s">
+        <v>103</v>
+      </c>
+      <c r="F44" t="s">
+        <v>134</v>
+      </c>
+      <c r="G44" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A45" s="78">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" t="s">
+        <v>81</v>
+      </c>
+      <c r="D45">
+        <v>160.59</v>
+      </c>
+      <c r="E45" t="s">
+        <v>107</v>
+      </c>
+      <c r="F45" t="s">
+        <v>180</v>
+      </c>
+      <c r="G45" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A46" s="78">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" t="s">
+        <v>81</v>
+      </c>
+      <c r="D46">
+        <v>215</v>
+      </c>
+      <c r="E46" t="s">
+        <v>161</v>
+      </c>
+      <c r="F46" t="s">
+        <v>162</v>
+      </c>
+      <c r="G46" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A47" s="78">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>139</v>
+      </c>
+      <c r="C47" t="s">
+        <v>140</v>
+      </c>
+      <c r="D47">
+        <v>149</v>
+      </c>
+      <c r="E47" t="s">
+        <v>62</v>
+      </c>
+      <c r="F47" t="s">
+        <v>146</v>
+      </c>
+      <c r="G47" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A48" s="78">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>139</v>
+      </c>
+      <c r="C48" t="s">
+        <v>140</v>
+      </c>
+      <c r="D48">
+        <v>149</v>
+      </c>
+      <c r="E48" t="s">
+        <v>103</v>
+      </c>
+      <c r="F48" t="s">
+        <v>151</v>
+      </c>
+      <c r="G48" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A49" s="78">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" t="s">
+        <v>84</v>
+      </c>
+      <c r="D49">
+        <v>289</v>
+      </c>
+      <c r="E49" t="s">
+        <v>62</v>
+      </c>
+      <c r="F49" t="s">
+        <v>85</v>
+      </c>
+      <c r="G49" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A50" s="78">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50" t="s">
+        <v>84</v>
+      </c>
+      <c r="D50">
+        <v>289</v>
+      </c>
+      <c r="E50" t="s">
+        <v>103</v>
+      </c>
+      <c r="F50" t="s">
+        <v>135</v>
+      </c>
+      <c r="G50" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created features in PreprocessedDataFrames file
</commit_message>
<xml_diff>
--- a/Estimator_Worksheet-1.xlsx
+++ b/Estimator_Worksheet-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kijah\Documents\Data_Bootcamp\Estimator_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC029E6C-E6BE-4797-B585-402F3DF23217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB4604F1-216E-4D1F-B654-1E1DF326D82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" firstSheet="17" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" firstSheet="19" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary - Rates" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,8 @@
     <sheet name="Cleaned_Data7" sheetId="20" r:id="rId20"/>
     <sheet name="Working_Table8" sheetId="21" r:id="rId21"/>
     <sheet name="Cleaned_Data8" sheetId="22" r:id="rId22"/>
+    <sheet name="Working_Table9" sheetId="23" r:id="rId23"/>
+    <sheet name="Cleaned_Data9" sheetId="24" r:id="rId24"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -55,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2932" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3224" uniqueCount="183">
   <si>
     <t>Sales Tax</t>
   </si>
@@ -602,6 +604,9 @@
   <si>
     <t>https://www.ebay.com/b/14-2-Romex-Indiana-OTHER-Industrial-Wires-Cables/92078/bn_7022085018</t>
   </si>
+  <si>
+    <t>11/07/2022 14:15:25</t>
+  </si>
 </sst>
 </file>
 
@@ -611,7 +616,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -807,6 +812,11 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -876,7 +886,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -1251,12 +1261,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1402,14 +1427,34 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="17" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1422,23 +1467,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9430,13 +9458,13 @@
       <c r="P8" s="63"/>
     </row>
     <row r="9" spans="1:16" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="89" t="s">
+      <c r="A9" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="80"/>
-      <c r="C9" s="80"/>
-      <c r="D9" s="80"/>
-      <c r="E9" s="90"/>
+      <c r="B9" s="81"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="82"/>
       <c r="F9" s="9"/>
       <c r="G9" s="51">
         <f t="shared" si="1"/>
@@ -9459,14 +9487,14 @@
         <v>11</v>
       </c>
       <c r="D10" s="14"/>
-      <c r="E10" s="91" t="s">
+      <c r="E10" s="83" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="54" t="str">
         <f>C10</f>
         <v>TOTAL</v>
       </c>
-      <c r="G10" s="93" t="s">
+      <c r="G10" s="85" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="63"/>
@@ -9486,11 +9514,11 @@
         <v>14</v>
       </c>
       <c r="D11" s="55"/>
-      <c r="E11" s="92"/>
+      <c r="E11" s="84"/>
       <c r="F11" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="82"/>
+      <c r="G11" s="86"/>
       <c r="H11" s="63"/>
       <c r="I11" s="63"/>
       <c r="J11" s="63"/>
@@ -9502,59 +9530,59 @@
       <c r="P11" s="63"/>
     </row>
     <row r="12" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="94" t="s">
+      <c r="A12" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="95">
+      <c r="B12" s="88">
         <f t="shared" ref="B12:G12" si="2">SUM(B2:B8)</f>
         <v>0</v>
       </c>
-      <c r="C12" s="95">
+      <c r="C12" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D12" s="95">
+      <c r="D12" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E12" s="95">
+      <c r="E12" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F12" s="95">
+      <c r="F12" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G12" s="83">
+      <c r="G12" s="91">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H12" s="85" t="s">
+      <c r="H12" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="82"/>
-      <c r="J12" s="82"/>
-      <c r="K12" s="82"/>
-      <c r="L12" s="82"/>
-      <c r="M12" s="82"/>
+      <c r="I12" s="86"/>
+      <c r="J12" s="86"/>
+      <c r="K12" s="86"/>
+      <c r="L12" s="86"/>
+      <c r="M12" s="86"/>
       <c r="N12" s="63"/>
       <c r="O12" s="63"/>
       <c r="P12" s="63"/>
     </row>
     <row r="13" spans="1:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="82"/>
-      <c r="B13" s="82"/>
-      <c r="C13" s="82"/>
-      <c r="D13" s="82"/>
-      <c r="E13" s="82"/>
-      <c r="F13" s="82"/>
-      <c r="G13" s="84"/>
-      <c r="H13" s="86"/>
-      <c r="I13" s="82"/>
-      <c r="J13" s="82"/>
-      <c r="K13" s="82"/>
-      <c r="L13" s="82"/>
-      <c r="M13" s="82"/>
+      <c r="A13" s="86"/>
+      <c r="B13" s="86"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="86"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="86"/>
+      <c r="G13" s="92"/>
+      <c r="H13" s="94"/>
+      <c r="I13" s="86"/>
+      <c r="J13" s="86"/>
+      <c r="K13" s="86"/>
+      <c r="L13" s="86"/>
+      <c r="M13" s="86"/>
       <c r="N13" s="63"/>
       <c r="O13" s="63"/>
       <c r="P13" s="63"/>
@@ -9619,10 +9647,10 @@
       <c r="B18" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="87"/>
-      <c r="D18" s="88"/>
-      <c r="E18" s="88"/>
-      <c r="F18" s="88"/>
+      <c r="C18" s="95"/>
+      <c r="D18" s="96"/>
+      <c r="E18" s="96"/>
+      <c r="F18" s="96"/>
       <c r="G18" s="63"/>
       <c r="H18" s="63"/>
       <c r="I18" s="63"/>
@@ -9639,10 +9667,10 @@
       <c r="B19" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="79"/>
-      <c r="D19" s="80"/>
-      <c r="E19" s="80"/>
-      <c r="F19" s="80"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="81"/>
+      <c r="F19" s="81"/>
       <c r="G19" s="63"/>
       <c r="H19" s="63"/>
       <c r="I19" s="63"/>
@@ -9659,15 +9687,15 @@
       <c r="B20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="87"/>
-      <c r="D20" s="88"/>
-      <c r="E20" s="88"/>
-      <c r="F20" s="88"/>
-      <c r="G20" s="88"/>
-      <c r="H20" s="88"/>
-      <c r="I20" s="88"/>
-      <c r="J20" s="88"/>
-      <c r="K20" s="88"/>
+      <c r="C20" s="95"/>
+      <c r="D20" s="96"/>
+      <c r="E20" s="96"/>
+      <c r="F20" s="96"/>
+      <c r="G20" s="96"/>
+      <c r="H20" s="96"/>
+      <c r="I20" s="96"/>
+      <c r="J20" s="96"/>
+      <c r="K20" s="96"/>
       <c r="L20" s="63"/>
       <c r="M20" s="63"/>
       <c r="N20" s="63"/>
@@ -9679,10 +9707,10 @@
       <c r="B21" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="79"/>
-      <c r="D21" s="80"/>
-      <c r="E21" s="80"/>
-      <c r="F21" s="80"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="81"/>
+      <c r="E21" s="81"/>
+      <c r="F21" s="81"/>
       <c r="G21" s="67"/>
       <c r="H21" s="63"/>
       <c r="I21" s="63"/>
@@ -9712,14 +9740,14 @@
     <row r="23" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A23" s="63"/>
       <c r="B23" s="63"/>
-      <c r="C23" s="81" t="s">
+      <c r="C23" s="90" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="82"/>
-      <c r="E23" s="82"/>
-      <c r="F23" s="82"/>
-      <c r="G23" s="82"/>
-      <c r="H23" s="82"/>
+      <c r="D23" s="86"/>
+      <c r="E23" s="86"/>
+      <c r="F23" s="86"/>
+      <c r="G23" s="86"/>
+      <c r="H23" s="86"/>
       <c r="I23" s="63"/>
       <c r="J23" s="63"/>
       <c r="K23" s="63"/>
@@ -9732,12 +9760,12 @@
     <row r="24" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A24" s="63"/>
       <c r="B24" s="63"/>
-      <c r="C24" s="82"/>
-      <c r="D24" s="82"/>
-      <c r="E24" s="82"/>
-      <c r="F24" s="82"/>
-      <c r="G24" s="82"/>
-      <c r="H24" s="82"/>
+      <c r="C24" s="86"/>
+      <c r="D24" s="86"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="86"/>
+      <c r="H24" s="86"/>
       <c r="I24" s="63"/>
       <c r="J24" s="63"/>
       <c r="K24" s="63"/>
@@ -9750,12 +9778,12 @@
     <row r="25" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A25" s="63"/>
       <c r="B25" s="63"/>
-      <c r="C25" s="82"/>
-      <c r="D25" s="82"/>
-      <c r="E25" s="82"/>
-      <c r="F25" s="82"/>
-      <c r="G25" s="82"/>
-      <c r="H25" s="82"/>
+      <c r="C25" s="86"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="86"/>
+      <c r="F25" s="86"/>
+      <c r="G25" s="86"/>
+      <c r="H25" s="86"/>
       <c r="I25" s="63"/>
       <c r="J25" s="63"/>
       <c r="K25" s="63"/>
@@ -9785,6 +9813,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C23:H25"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:M13"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:K20"/>
     <mergeCell ref="A9:E9"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="G10:G11"/>
@@ -9794,13 +9829,6 @@
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C23:H25"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:M13"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:K20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11439,7 +11467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:G50"/>
     </sheetView>
   </sheetViews>
@@ -12599,6 +12627,1382 @@
       </c>
       <c r="G50" t="s">
         <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.9296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="110.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B1" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="79" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="79" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="79" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" s="79" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="79" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" s="79">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" s="79">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3">
+        <v>8.6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" s="79">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4">
+        <v>17.55</v>
+      </c>
+      <c r="E4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" s="79">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5">
+        <v>3.98</v>
+      </c>
+      <c r="E5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" s="79">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6">
+        <v>2.98</v>
+      </c>
+      <c r="E6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" s="79">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" s="79">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8">
+        <v>8.5399999999999991</v>
+      </c>
+      <c r="E8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" s="79">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" t="s">
+        <v>148</v>
+      </c>
+      <c r="G9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" s="79">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10">
+        <v>1.6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" t="s">
+        <v>120</v>
+      </c>
+      <c r="G10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" s="79">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11">
+        <v>84.99</v>
+      </c>
+      <c r="E11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" s="79">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12">
+        <v>158</v>
+      </c>
+      <c r="E12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" t="s">
+        <v>82</v>
+      </c>
+      <c r="G12" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" s="79">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" t="s">
+        <v>140</v>
+      </c>
+      <c r="D13">
+        <v>149</v>
+      </c>
+      <c r="E13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" t="s">
+        <v>146</v>
+      </c>
+      <c r="G13" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" s="79">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14">
+        <v>279</v>
+      </c>
+      <c r="E14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" s="79">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15">
+        <v>60</v>
+      </c>
+      <c r="E15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" s="79">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16">
+        <v>106</v>
+      </c>
+      <c r="E16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" t="s">
+        <v>91</v>
+      </c>
+      <c r="G16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" s="79">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17">
+        <v>155.99</v>
+      </c>
+      <c r="E17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" t="s">
+        <v>94</v>
+      </c>
+      <c r="G17" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+  <dimension ref="A1:G41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.9296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="114.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B1" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="79" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="79" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="79" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" s="79" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="79" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" s="79">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2">
+        <v>20.62</v>
+      </c>
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" s="79">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3">
+        <v>17.55</v>
+      </c>
+      <c r="E3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" s="79">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4">
+        <v>11.91</v>
+      </c>
+      <c r="E4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" s="79">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5">
+        <v>10.47</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" s="79">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6">
+        <v>8.6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" s="79">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7">
+        <v>8.5399999999999991</v>
+      </c>
+      <c r="E7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" s="79">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" s="79">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" s="79">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10">
+        <v>3.98</v>
+      </c>
+      <c r="E10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" t="s">
+        <v>102</v>
+      </c>
+      <c r="G10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" s="79">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11">
+        <v>8.5399999999999991</v>
+      </c>
+      <c r="E11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" s="79">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" t="s">
+        <v>117</v>
+      </c>
+      <c r="G12" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" s="79">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13">
+        <v>5.99</v>
+      </c>
+      <c r="E13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F13" t="s">
+        <v>118</v>
+      </c>
+      <c r="G13" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" s="79">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14">
+        <v>11.03</v>
+      </c>
+      <c r="E14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" t="s">
+        <v>148</v>
+      </c>
+      <c r="G14" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" s="79">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15">
+        <v>6.45</v>
+      </c>
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" t="s">
+        <v>177</v>
+      </c>
+      <c r="G15" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" s="79">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16">
+        <v>1.6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" t="s">
+        <v>120</v>
+      </c>
+      <c r="G16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" s="79">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17">
+        <v>2.98</v>
+      </c>
+      <c r="E17" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" s="79">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18">
+        <v>5.99</v>
+      </c>
+      <c r="E18" t="s">
+        <v>103</v>
+      </c>
+      <c r="F18" t="s">
+        <v>121</v>
+      </c>
+      <c r="G18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" s="79">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19">
+        <v>2.98</v>
+      </c>
+      <c r="E19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F19" t="s">
+        <v>150</v>
+      </c>
+      <c r="G19" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20" s="79">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20">
+        <v>81.95</v>
+      </c>
+      <c r="E20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" t="s">
+        <v>122</v>
+      </c>
+      <c r="G20" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" s="79">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21">
+        <v>75.989999999999995</v>
+      </c>
+      <c r="E21" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" s="79">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22">
+        <v>80</v>
+      </c>
+      <c r="E22" t="s">
+        <v>127</v>
+      </c>
+      <c r="F22" t="s">
+        <v>156</v>
+      </c>
+      <c r="G22" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23" s="79">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23">
+        <v>60</v>
+      </c>
+      <c r="E23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" t="s">
+        <v>165</v>
+      </c>
+      <c r="G23" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A24" s="79">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24">
+        <v>64.989999999999995</v>
+      </c>
+      <c r="E24" t="s">
+        <v>157</v>
+      </c>
+      <c r="F24" t="s">
+        <v>158</v>
+      </c>
+      <c r="G24" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A25" s="79">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25">
+        <v>106</v>
+      </c>
+      <c r="E25" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" t="s">
+        <v>124</v>
+      </c>
+      <c r="G25" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A26" s="79">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" t="s">
+        <v>90</v>
+      </c>
+      <c r="D26">
+        <v>109</v>
+      </c>
+      <c r="E26" t="s">
+        <v>103</v>
+      </c>
+      <c r="F26" t="s">
+        <v>125</v>
+      </c>
+      <c r="G26" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A27" s="79">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27">
+        <v>114.95</v>
+      </c>
+      <c r="E27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" t="s">
+        <v>91</v>
+      </c>
+      <c r="G27" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A28" s="79">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28">
+        <v>156</v>
+      </c>
+      <c r="E28" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" t="s">
+        <v>126</v>
+      </c>
+      <c r="G28" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A29" s="79">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29">
+        <v>155.99</v>
+      </c>
+      <c r="E29" t="s">
+        <v>58</v>
+      </c>
+      <c r="F29" t="s">
+        <v>94</v>
+      </c>
+      <c r="G29" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A30" s="79">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" t="s">
+        <v>93</v>
+      </c>
+      <c r="D30">
+        <v>165</v>
+      </c>
+      <c r="E30" t="s">
+        <v>127</v>
+      </c>
+      <c r="F30" t="s">
+        <v>128</v>
+      </c>
+      <c r="G30" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A31" s="79">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31">
+        <v>118</v>
+      </c>
+      <c r="E31" t="s">
+        <v>58</v>
+      </c>
+      <c r="F31" t="s">
+        <v>79</v>
+      </c>
+      <c r="G31" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A32" s="79">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" t="s">
+        <v>78</v>
+      </c>
+      <c r="D32">
+        <v>118</v>
+      </c>
+      <c r="E32" t="s">
+        <v>103</v>
+      </c>
+      <c r="F32" t="s">
+        <v>145</v>
+      </c>
+      <c r="G32" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A33" s="79">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" t="s">
+        <v>78</v>
+      </c>
+      <c r="D33">
+        <v>111.07</v>
+      </c>
+      <c r="E33" t="s">
+        <v>107</v>
+      </c>
+      <c r="F33" t="s">
+        <v>129</v>
+      </c>
+      <c r="G33" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A34" s="79">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34">
+        <v>84.99</v>
+      </c>
+      <c r="E34" t="s">
+        <v>130</v>
+      </c>
+      <c r="F34" t="s">
+        <v>131</v>
+      </c>
+      <c r="G34" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A35" s="79">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" t="s">
+        <v>81</v>
+      </c>
+      <c r="D35">
+        <v>158</v>
+      </c>
+      <c r="E35" t="s">
+        <v>62</v>
+      </c>
+      <c r="F35" t="s">
+        <v>82</v>
+      </c>
+      <c r="G35" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A36" s="79">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" t="s">
+        <v>81</v>
+      </c>
+      <c r="D36">
+        <v>159</v>
+      </c>
+      <c r="E36" t="s">
+        <v>103</v>
+      </c>
+      <c r="F36" t="s">
+        <v>134</v>
+      </c>
+      <c r="G36" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A37" s="79">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37">
+        <v>215</v>
+      </c>
+      <c r="E37" t="s">
+        <v>161</v>
+      </c>
+      <c r="F37" t="s">
+        <v>162</v>
+      </c>
+      <c r="G37" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A38" s="79">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>139</v>
+      </c>
+      <c r="C38" t="s">
+        <v>140</v>
+      </c>
+      <c r="D38">
+        <v>149</v>
+      </c>
+      <c r="E38" t="s">
+        <v>62</v>
+      </c>
+      <c r="F38" t="s">
+        <v>146</v>
+      </c>
+      <c r="G38" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A39" s="79">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>139</v>
+      </c>
+      <c r="C39" t="s">
+        <v>140</v>
+      </c>
+      <c r="D39">
+        <v>149</v>
+      </c>
+      <c r="E39" t="s">
+        <v>103</v>
+      </c>
+      <c r="F39" t="s">
+        <v>151</v>
+      </c>
+      <c r="G39" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A40" s="79">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40">
+        <v>289</v>
+      </c>
+      <c r="E40" t="s">
+        <v>62</v>
+      </c>
+      <c r="F40" t="s">
+        <v>85</v>
+      </c>
+      <c r="G40" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A41" s="79">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" t="s">
+        <v>84</v>
+      </c>
+      <c r="D41">
+        <v>279</v>
+      </c>
+      <c r="E41" t="s">
+        <v>103</v>
+      </c>
+      <c r="F41" t="s">
+        <v>135</v>
+      </c>
+      <c r="G41" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>